<commit_message>
import and export excel
</commit_message>
<xml_diff>
--- a/documents/功能进度计划.xlsx
+++ b/documents/功能进度计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
   <si>
     <t>需求名称</t>
   </si>
@@ -238,10 +238,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>开发工作流，并且有demo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">
 /services/sys/resourcesService/findResourcesSiteMenu没有开发路径应该是404
 加请求头验证
@@ -326,6 +322,44 @@
   </si>
   <si>
     <t>开发start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缓存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icustom.api.test.ui</t>
+  </si>
+  <si>
+    <t>类似Google Advanced REST Client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发责任人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试责任人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aGuang</t>
+  </si>
+  <si>
+    <t>aGuang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发工作流(activiti)，并且有demo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -570,7 +604,283 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -764,6 +1074,68 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -894,6 +1266,23 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -919,299 +1308,6 @@
         <bottom/>
       </border>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1224,36 +1320,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I31" totalsRowShown="0" headerRowDxfId="11" dataDxfId="21">
-  <autoFilter ref="A1:I31"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="序列" dataDxfId="20"/>
-    <tableColumn id="2" name="需求名称" dataDxfId="19"/>
-    <tableColumn id="3" name="优先级别" dataDxfId="18"/>
-    <tableColumn id="4" name="完成状态" dataDxfId="17"/>
-    <tableColumn id="5" name="计划类型" dataDxfId="16"/>
-    <tableColumn id="6" name="功能维度" dataDxfId="15"/>
-    <tableColumn id="7" name="计划日期" dataDxfId="14"/>
-    <tableColumn id="8" name="完成日期" dataDxfId="13"/>
-    <tableColumn id="9" name="补充说明" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K33" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:K33">
+    <filterColumn colId="5"/>
+    <filterColumn colId="6"/>
+  </autoFilter>
+  <tableColumns count="11">
+    <tableColumn id="1" name="序列" dataDxfId="21"/>
+    <tableColumn id="2" name="需求名称" dataDxfId="20"/>
+    <tableColumn id="3" name="优先级别" dataDxfId="19"/>
+    <tableColumn id="4" name="完成状态" dataDxfId="18"/>
+    <tableColumn id="5" name="计划类型" dataDxfId="17"/>
+    <tableColumn id="10" name="开发" dataDxfId="16"/>
+    <tableColumn id="11" name="测试" dataDxfId="15"/>
+    <tableColumn id="6" name="功能维度" dataDxfId="14"/>
+    <tableColumn id="7" name="计划日期" dataDxfId="13"/>
+    <tableColumn id="8" name="完成日期" dataDxfId="12"/>
+    <tableColumn id="9" name="补充说明" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I4"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="序列" dataDxfId="10"/>
-    <tableColumn id="2" name="需求名称" dataDxfId="9"/>
-    <tableColumn id="3" name="优先级别" dataDxfId="8"/>
-    <tableColumn id="4" name="完成状态" dataDxfId="7"/>
-    <tableColumn id="5" name="计划类型" dataDxfId="6"/>
-    <tableColumn id="6" name="功能维度" dataDxfId="5"/>
-    <tableColumn id="7" name="计划日期" dataDxfId="4"/>
-    <tableColumn id="8" name="完成日期" dataDxfId="3"/>
-    <tableColumn id="9" name="补充说明" dataDxfId="2"/>
+    <tableColumn id="1" name="序列" dataDxfId="8"/>
+    <tableColumn id="2" name="需求名称" dataDxfId="7"/>
+    <tableColumn id="3" name="优先级别" dataDxfId="6"/>
+    <tableColumn id="4" name="完成状态" dataDxfId="5"/>
+    <tableColumn id="5" name="计划类型" dataDxfId="4"/>
+    <tableColumn id="6" name="功能维度" dataDxfId="3"/>
+    <tableColumn id="7" name="计划日期" dataDxfId="2"/>
+    <tableColumn id="8" name="完成日期" dataDxfId="1"/>
+    <tableColumn id="9" name="补充说明" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1544,11 +1645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
@@ -1557,17 +1658,17 @@
     <col min="2" max="2" width="41.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="13.25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="53.875" style="1" customWidth="1"/>
-    <col min="10" max="13" width="9" style="1"/>
-    <col min="14" max="14" width="15.625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="5" max="8" width="13.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="53.875" style="1" customWidth="1"/>
+    <col min="12" max="15" width="9" style="1"/>
+    <col min="16" max="16" width="15.625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="24.75" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
@@ -1584,19 +1685,25 @@
         <v>6</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="24.75" customHeight="1">
+    <row r="2" spans="1:18" ht="24.75" customHeight="1">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1609,19 +1716,31 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
       <c r="I2" s="13"/>
-      <c r="L2" s="1" t="s">
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="N2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="24.75" customHeight="1">
+      <c r="Q2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="24.75" customHeight="1">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1633,23 +1752,28 @@
         <v>20</v>
       </c>
       <c r="E3" s="13"/>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
       <c r="I3" s="13"/>
-      <c r="L3" s="4" t="s">
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="N3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="3">
-        <v>42879</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="24.75" customHeight="1">
+      <c r="Q3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="24.75" customHeight="1">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1661,20 +1785,22 @@
         <v>20</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
       <c r="I4" s="13"/>
-      <c r="L4" s="5" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="N4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="24.75" customHeight="1">
+    <row r="5" spans="1:18" ht="24.75" customHeight="1">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1686,20 +1812,22 @@
         <v>20</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
       <c r="I5" s="13"/>
-      <c r="L5" s="1" t="s">
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="N5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="24.75" customHeight="1">
+    <row r="6" spans="1:18" ht="24.75" customHeight="1">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1711,17 +1839,19 @@
         <v>20</v>
       </c>
       <c r="E6" s="13"/>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
       <c r="I6" s="13"/>
-      <c r="L6" s="7" t="s">
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="N6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="24.75" customHeight="1">
+    <row r="7" spans="1:18" ht="24.75" customHeight="1">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1733,19 +1863,21 @@
         <v>20</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" s="8" t="s">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="24.75" customHeight="1">
+    <row r="8" spans="1:18" ht="24.75" customHeight="1">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1757,19 +1889,21 @@
         <v>8</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
       <c r="I8" s="13"/>
-      <c r="L8" s="10" t="s">
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="N8" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="24.75" customHeight="1">
+    <row r="9" spans="1:18" ht="24.75" customHeight="1">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1785,11 +1919,13 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
-      <c r="L9" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="24.75" customHeight="1">
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="N9" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="24.75" customHeight="1">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -1798,20 +1934,22 @@
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="L10" s="9" t="s">
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="N10" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="24.75" customHeight="1">
+    <row r="11" spans="1:18" ht="24.75" customHeight="1">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -1827,11 +1965,13 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="L11" s="6" t="s">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="N11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="24.75" customHeight="1">
+    <row r="12" spans="1:18" ht="24.75" customHeight="1">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -1843,14 +1983,16 @@
         <v>8</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="1:15" ht="24.75" customHeight="1">
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="13" spans="1:18" ht="24.75" customHeight="1">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -1862,14 +2004,16 @@
         <v>28</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:15" ht="24.75" customHeight="1">
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+    </row>
+    <row r="14" spans="1:18" ht="24.75" customHeight="1">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -1878,15 +2022,17 @@
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="1:15" ht="24.75" customHeight="1">
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+    </row>
+    <row r="15" spans="1:18" ht="24.75" customHeight="1">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1895,15 +2041,17 @@
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:15" ht="24.75" customHeight="1">
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+    </row>
+    <row r="16" spans="1:18" ht="24.75" customHeight="1">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -1919,8 +2067,10 @@
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="1:9" ht="24.75" customHeight="1">
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" ht="24.75" customHeight="1">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -1932,14 +2082,16 @@
         <v>28</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="1:9" ht="24.75" customHeight="1">
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18" spans="1:11" ht="24.75" customHeight="1">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -1951,14 +2103,16 @@
         <v>9</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="1:9" ht="24.75" customHeight="1">
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" ht="24.75" customHeight="1">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -1970,120 +2124,132 @@
         <v>9</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="1:9" ht="24.75" customHeight="1">
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="1:11" ht="24.75" customHeight="1">
       <c r="A20" s="18">
         <v>19</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="24.75" customHeight="1">
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="24.75" customHeight="1">
       <c r="A21" s="12">
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="24.75" customHeight="1">
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="24.75" customHeight="1">
       <c r="A22" s="18">
         <v>21</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="24.75" customHeight="1">
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="24.75" customHeight="1">
       <c r="A23" s="12">
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="1:9" ht="24.75" customHeight="1">
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="1:11" ht="24.75" customHeight="1">
       <c r="A24" s="12">
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
-    </row>
-    <row r="25" spans="1:9" ht="24.75" customHeight="1">
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="25" spans="1:11" ht="24.75" customHeight="1">
       <c r="A25" s="12">
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13" t="s">
@@ -2094,13 +2260,15 @@
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
-    </row>
-    <row r="26" spans="1:9" ht="24.75" customHeight="1">
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" ht="24.75" customHeight="1">
       <c r="A26" s="12">
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13" t="s">
@@ -2111,72 +2279,80 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
-    </row>
-    <row r="27" spans="1:9" ht="24.75" customHeight="1">
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" spans="1:11" ht="24.75" customHeight="1">
       <c r="A27" s="18">
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+        <v>56</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="24.75" customHeight="1">
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="24.75" customHeight="1">
       <c r="A28" s="12">
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
-    </row>
-    <row r="29" spans="1:9" ht="24.75" customHeight="1">
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+    </row>
+    <row r="29" spans="1:11" ht="24.75" customHeight="1">
       <c r="A29" s="12">
         <v>28</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
         <v>28</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
-      <c r="I29" s="22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="24.75" customHeight="1">
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="24.75" customHeight="1">
       <c r="A30" s="20"/>
       <c r="B30" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -2184,12 +2360,14 @@
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
-      <c r="I30" s="22"/>
-    </row>
-    <row r="31" spans="1:9" ht="24.75" customHeight="1">
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="31" spans="1:11" ht="24.75" customHeight="1">
       <c r="A31" s="20"/>
       <c r="B31" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -2197,31 +2375,49 @@
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
-      <c r="I31" s="22"/>
-    </row>
-    <row r="32" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-    </row>
-    <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-    </row>
-    <row r="34" spans="1:9" ht="24.75" customHeight="1">
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="22"/>
+    </row>
+    <row r="32" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A32" s="20"/>
+      <c r="B32" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="22"/>
+    </row>
+    <row r="33" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A33" s="20"/>
+      <c r="B33" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="24.75" customHeight="1">
       <c r="A34" s="12"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -2231,15 +2427,23 @@
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E31">
-      <formula1>$N$3:$N$5</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E33">
+      <formula1>$P$3:$P$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
-      <formula1>$L$3:$L$11</formula1>
+      <formula1>$N$3:$N$11</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+      <formula1>$Q$3:$Q$11</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+      <formula1>$R$3:$R$11</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2309,13 +2513,13 @@
         <v>20</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5">
@@ -2323,20 +2527,20 @@
         <v>26</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.5">
@@ -2344,14 +2548,14 @@
         <v>27</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>

</xml_diff>

<commit_message>
add html area module
</commit_message>
<xml_diff>
--- a/documents/功能进度计划.xlsx
+++ b/documents/功能进度计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="86">
   <si>
     <t>需求名称</t>
   </si>
@@ -369,6 +369,25 @@
   </si>
   <si>
     <t>公共缓存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>富文本模块-通过URL替换CSS\HTML\JS等内容,不用重新发包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础组件开发</t>
+  </si>
+  <si>
+    <t>基础组件开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lookup 数据列表开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cxf  java配置方式多个模块的配置不能并存</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -511,17 +530,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -543,6 +551,19 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -615,19 +636,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1350,8 +1371,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K33" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:K33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K36" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:K36">
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
   </autoFilter>
@@ -1675,11 +1696,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="B27:E27"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
@@ -1868,7 +1889,9 @@
       <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13" t="s">
@@ -1880,16 +1903,19 @@
       <c r="N6" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="P6" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="1:18" ht="24.75" customHeight="1">
       <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="13" t="s">
@@ -1911,14 +1937,14 @@
       <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>51</v>
       </c>
       <c r="F8" s="13"/>
@@ -1928,7 +1954,7 @@
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="21" t="s">
         <v>67</v>
       </c>
       <c r="N8" s="10" t="s">
@@ -1969,7 +1995,7 @@
         <v>28</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
@@ -1994,7 +2020,9 @@
       <c r="D11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -2030,14 +2058,14 @@
       <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24" t="s">
+      <c r="C13" s="23"/>
+      <c r="D13" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="13"/>
@@ -2096,7 +2124,9 @@
       <c r="D16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -2225,7 +2255,7 @@
         <v>28</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
@@ -2248,7 +2278,7 @@
         <v>9</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -2364,99 +2394,115 @@
       <c r="A29" s="12">
         <v>28</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21" t="s">
+      <c r="C29" s="20"/>
+      <c r="D29" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="22" t="s">
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21" t="s">
+      <c r="A30" s="12">
+        <v>29</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21" t="s">
+      <c r="C30" s="20"/>
+      <c r="D30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="22"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="21"/>
     </row>
     <row r="31" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A31" s="20"/>
-      <c r="B31" s="21" t="s">
+      <c r="A31" s="12">
+        <v>30</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21" t="s">
+      <c r="C31" s="20"/>
+      <c r="D31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="22"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="21"/>
     </row>
     <row r="32" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21" t="s">
+      <c r="A32" s="12">
+        <v>31</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21" t="s">
+      <c r="C32" s="20"/>
+      <c r="D32" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="22"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="21"/>
     </row>
     <row r="33" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="21" t="s">
+      <c r="A33" s="12">
+        <v>32</v>
+      </c>
+      <c r="B33" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="22" t="s">
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
+      <c r="A34" s="12">
+        <v>33</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>81</v>
+      </c>
       <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
+      <c r="D34" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
@@ -2464,11 +2510,79 @@
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
     </row>
+    <row r="35" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A35" s="12">
+        <v>34</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="24"/>
+    </row>
+    <row r="36" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A36" s="12">
+        <v>35</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="24"/>
+    </row>
+    <row r="37" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+    </row>
+    <row r="38" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A38" s="12"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E33">
-      <formula1>$P$3:$P$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+      <formula1>$P$3:$P$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>$N$3:$N$11</formula1>

</xml_diff>

<commit_message>
excel and html area module
</commit_message>
<xml_diff>
--- a/documents/功能进度计划.xlsx
+++ b/documents/功能进度计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
   <si>
     <t>需求名称</t>
   </si>
@@ -388,6 +388,10 @@
   </si>
   <si>
     <t>cxf  java配置方式多个模块的配置不能并存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>security 4 增加当前用户接口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1371,8 +1375,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K36" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:K36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K37" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:K37">
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
   </autoFilter>
@@ -1700,13 +1704,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" style="11"/>
-    <col min="2" max="2" width="41.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
     <col min="5" max="8" width="13.25" style="1" customWidth="1"/>
@@ -2553,17 +2557,25 @@
       <c r="K36" s="24"/>
     </row>
     <row r="37" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A37" s="12"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
+      <c r="A37" s="12">
+        <v>36</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="21"/>
     </row>
     <row r="38" spans="1:11" ht="24.75" customHeight="1">
       <c r="A38" s="12"/>

</xml_diff>

<commit_message>
html area page update
</commit_message>
<xml_diff>
--- a/documents/功能进度计划.xlsx
+++ b/documents/功能进度计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="87">
   <si>
     <t>需求名称</t>
   </si>
@@ -202,10 +202,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>文件上传下载组件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>导入导出excel组件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -223,10 +219,6 @@
   </si>
   <si>
     <t>国际化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>写一个页面JS分页插件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -263,10 +255,6 @@
     <t>待增加功能</t>
   </si>
   <si>
-    <t>icustom metrics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>icustom redis</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -344,10 +332,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>开发工作流(activiti)，并且有demo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>测试start pom</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -392,6 +376,22 @@
   </si>
   <si>
     <t>security 4 增加当前用户接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件管理,文件上传下载组件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写一个 JS分页插件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icustom metrics  监控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icustom.activiti 工作流开发，并且有demo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -510,7 +510,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -570,13 +570,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -655,6 +666,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1375,8 +1389,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K37" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:K37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K38" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:K38">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="待续"/>
+        <filter val="加急优先"/>
+        <filter val="进行中"/>
+        <filter val="马上进行"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
   </autoFilter>
@@ -1703,8 +1725,8 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23:D24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
@@ -1740,10 +1762,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>30</v>
@@ -1758,7 +1780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="24.75" customHeight="1">
+    <row r="2" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1771,10 +1793,10 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>32</v>
@@ -1789,13 +1811,13 @@
         <v>6</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="24.75" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1822,13 +1844,13 @@
         <v>12</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="24.75" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1855,7 +1877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="24.75" customHeight="1">
+    <row r="5" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1882,7 +1904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="24.75" customHeight="1">
+    <row r="6" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1894,7 +1916,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -1908,10 +1930,10 @@
         <v>16</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="24.75" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1923,7 +1945,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -1931,7 +1953,7 @@
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N7" s="8" t="s">
         <v>17</v>
@@ -1949,7 +1971,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -1959,7 +1981,7 @@
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N8" s="10" t="s">
         <v>21</v>
@@ -1976,7 +1998,9 @@
       <c r="D9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -1984,22 +2008,22 @@
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="N9" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="24.75" customHeight="1">
       <c r="A10" s="18">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>82</v>
+      <c r="B10" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
@@ -2007,13 +2031,13 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N10" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="24.75" customHeight="1">
+    <row r="11" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -2025,7 +2049,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -2042,14 +2066,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
@@ -2063,14 +2087,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -2079,16 +2103,16 @@
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:18" ht="24.75" customHeight="1">
+    <row r="14" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A14" s="12">
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -2098,16 +2122,16 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:18" ht="24.75" customHeight="1">
+    <row r="15" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A15" s="12">
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -2117,19 +2141,19 @@
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="1:18" ht="24.75" customHeight="1">
+    <row r="16" spans="1:18" ht="24.75" hidden="1" customHeight="1">
       <c r="A16" s="12">
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -2143,14 +2167,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -2164,14 +2188,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -2185,14 +2209,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -2201,19 +2225,19 @@
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="1:11" ht="24.75" customHeight="1">
+    <row r="20" spans="1:11" ht="24.75" hidden="1" customHeight="1">
       <c r="A20" s="18">
         <v>19</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19" t="s">
         <v>20</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
@@ -2221,7 +2245,7 @@
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="24.75" customHeight="1">
@@ -2229,14 +2253,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -2244,7 +2268,7 @@
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="24.75" customHeight="1">
@@ -2252,14 +2276,14 @@
         <v>21</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
@@ -2267,7 +2291,7 @@
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="24.75" customHeight="1">
@@ -2275,14 +2299,14 @@
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -2296,14 +2320,14 @@
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -2317,7 +2341,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13" t="s">
@@ -2336,7 +2360,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13" t="s">
@@ -2355,14 +2379,14 @@
         <v>26</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
@@ -2370,22 +2394,22 @@
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="24.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="24.75" hidden="1" customHeight="1">
       <c r="A28" s="12">
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
@@ -2399,14 +2423,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
@@ -2414,7 +2438,7 @@
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
       <c r="K29" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1">
@@ -2422,7 +2446,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="20" t="s">
@@ -2436,16 +2460,16 @@
       <c r="J30" s="20"/>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="1:11" ht="24.75" customHeight="1">
+    <row r="31" spans="1:11" ht="24.75" hidden="1" customHeight="1">
       <c r="A31" s="12">
         <v>30</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="20" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
@@ -2460,13 +2484,15 @@
         <v>31</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="20"/>
+        <v>26</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -2479,18 +2505,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
+      <c r="D33" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>50</v>
+      </c>
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
       <c r="K33" s="21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="24.75" customHeight="1">
@@ -2498,14 +2528,14 @@
         <v>33</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
@@ -2514,19 +2544,19 @@
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" ht="24.75" customHeight="1">
+    <row r="35" spans="1:11" ht="24.75" hidden="1" customHeight="1">
       <c r="A35" s="12">
         <v>34</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
@@ -2540,14 +2570,14 @@
         <v>35</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="16" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="20"/>
@@ -2561,14 +2591,14 @@
         <v>36</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C37" s="20"/>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="16" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
@@ -2578,17 +2608,25 @@
       <c r="K37" s="21"/>
     </row>
     <row r="38" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
+      <c r="A38" s="25">
+        <v>37</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2673,13 +2711,13 @@
         <v>20</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5">
@@ -2687,20 +2725,20 @@
         <v>26</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.5">
@@ -2708,14 +2746,14 @@
         <v>27</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>

</xml_diff>